<commit_message>
feat: update sheets for 2024-02
</commit_message>
<xml_diff>
--- a/资产负债表.xlsx
+++ b/资产负债表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\finance\recording\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C0F1A4-E3A5-4E03-A011-0971D524D947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF4ED9F-2374-4BD7-90BA-B177C16BD679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="285" windowWidth="29040" windowHeight="15615" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -323,6 +323,9 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="176" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -331,9 +334,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -532,9 +532,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>(个人现金流量及资产负债表!$D$1:$O$1,个人现金流量及资产负债表!$Q$1:$AB$1,个人现金流量及资产负债表!$AD$1:$AO$1,个人现金流量及资产负债表!$AQ$1:$BB$1,个人现金流量及资产负债表!$BD$1:$BO$1,个人现金流量及资产负债表!$BQ$1:$BQ$1)</c:f>
+              <c:f>(个人现金流量及资产负债表!$D$1:$O$1,个人现金流量及资产负债表!$Q$1:$AB$1,个人现金流量及资产负债表!$AD$1:$AO$1,个人现金流量及资产负债表!$AQ$1:$BB$1,个人现金流量及资产负债表!$BD$1:$BO$1,个人现金流量及资产负债表!$BQ$1:$BR$1)</c:f>
               <c:strCache>
-                <c:ptCount val="61"/>
+                <c:ptCount val="62"/>
                 <c:pt idx="0">
                   <c:v>2019/01</c:v>
                 </c:pt>
@@ -717,16 +717,19 @@
                 </c:pt>
                 <c:pt idx="60">
                   <c:v>2024/01</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2024/02</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(个人现金流量及资产负债表!$D$23:$O$23,个人现金流量及资产负债表!$Q$23:$AB$23,个人现金流量及资产负债表!$AD$23:$AO$23,个人现金流量及资产负债表!$AQ$23:$BB$23,个人现金流量及资产负债表!$BD$23:$BO$23,个人现金流量及资产负债表!$BQ$23:$BQ$23)</c:f>
+              <c:f>(个人现金流量及资产负债表!$D$23:$O$23,个人现金流量及资产负债表!$Q$23:$AB$23,个人现金流量及资产负债表!$AD$23:$AO$23,个人现金流量及资产负债表!$AQ$23:$BB$23,个人现金流量及资产负债表!$BD$23:$BO$23,个人现金流量及资产负债表!$BQ$23:$BR$23)</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="61"/>
+                <c:ptCount val="62"/>
                 <c:pt idx="0">
                   <c:v>96624.5</c:v>
                 </c:pt>
@@ -909,6 +912,9 @@
                 </c:pt>
                 <c:pt idx="60">
                   <c:v>745879.6</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>799043.04</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -979,9 +985,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>(个人现金流量及资产负债表!$D$1:$O$1,个人现金流量及资产负债表!$Q$1:$AB$1,个人现金流量及资产负债表!$AD$1:$AO$1,个人现金流量及资产负债表!$AQ$1:$BB$1,个人现金流量及资产负债表!$BD$1:$BO$1,个人现金流量及资产负债表!$BQ$1:$BQ$1)</c:f>
+              <c:f>(个人现金流量及资产负债表!$D$1:$O$1,个人现金流量及资产负债表!$Q$1:$AB$1,个人现金流量及资产负债表!$AD$1:$AO$1,个人现金流量及资产负债表!$AQ$1:$BB$1,个人现金流量及资产负债表!$BD$1:$BO$1,个人现金流量及资产负债表!$BQ$1:$BR$1)</c:f>
               <c:strCache>
-                <c:ptCount val="61"/>
+                <c:ptCount val="62"/>
                 <c:pt idx="0">
                   <c:v>2019/01</c:v>
                 </c:pt>
@@ -1164,16 +1170,19 @@
                 </c:pt>
                 <c:pt idx="60">
                   <c:v>2024/01</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2024/02</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(个人现金流量及资产负债表!$D$25:$O$25,个人现金流量及资产负债表!$Q$25:$AB$25,个人现金流量及资产负债表!$AD$25:$AO$25,个人现金流量及资产负债表!$AQ$25:$BB$25,个人现金流量及资产负债表!$BD$25:$BO$25,个人现金流量及资产负债表!$BQ$25:$BQ$25)</c:f>
+              <c:f>(个人现金流量及资产负债表!$D$25:$O$25,个人现金流量及资产负债表!$Q$25:$AB$25,个人现金流量及资产负债表!$AD$25:$AO$25,个人现金流量及资产负债表!$AQ$25:$BB$25,个人现金流量及资产负债表!$BD$25:$BO$25,个人现金流量及资产负债表!$BQ$25:$BR$25)</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="61"/>
+                <c:ptCount val="62"/>
                 <c:pt idx="0">
                   <c:v>39892.050000000003</c:v>
                 </c:pt>
@@ -1356,6 +1365,9 @@
                 </c:pt>
                 <c:pt idx="60">
                   <c:v>589879.6</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>643043.04</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1616,13 +1628,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>70</xdr:col>
+      <xdr:col>71</xdr:col>
       <xdr:colOff>723900</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>77</xdr:col>
+      <xdr:col>78</xdr:col>
       <xdr:colOff>47805</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>63630</xdr:rowOff>
@@ -1911,11 +1923,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:ANV25"/>
+  <dimension ref="A1:ANW25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" topLeftCell="BI1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BR8" sqref="BR8"/>
+      <selection pane="topRight" activeCell="BS26" sqref="BS26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1934,18 +1946,18 @@
     <col min="55" max="55" width="12.25" style="3" customWidth="1"/>
     <col min="56" max="67" width="10.5" style="3" customWidth="1"/>
     <col min="68" max="68" width="12.25" style="3" customWidth="1"/>
-    <col min="69" max="69" width="10.5" style="3" customWidth="1"/>
-    <col min="70" max="70" width="12.25" style="3" customWidth="1"/>
-    <col min="71" max="106" width="10.5" style="3" customWidth="1"/>
-    <col min="107" max="1062" width="10.5" style="2" customWidth="1"/>
+    <col min="69" max="70" width="10.5" style="3" customWidth="1"/>
+    <col min="71" max="71" width="12.25" style="3" customWidth="1"/>
+    <col min="72" max="107" width="10.5" style="3" customWidth="1"/>
+    <col min="108" max="1063" width="10.5" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1062" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
+    <row r="1" spans="1:1063" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
       <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
@@ -2144,10 +2156,12 @@
       <c r="BQ1" s="4">
         <v>45292</v>
       </c>
-      <c r="BR1" s="14" t="s">
+      <c r="BR1" s="4">
+        <v>45323</v>
+      </c>
+      <c r="BS1" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="BS1" s="10"/>
       <c r="BT1" s="10"/>
       <c r="BU1" s="10"/>
       <c r="BV1" s="10"/>
@@ -3139,12 +3153,13 @@
       <c r="ANT1" s="10"/>
       <c r="ANU1" s="10"/>
       <c r="ANV1" s="10"/>
+      <c r="ANW1" s="10"/>
     </row>
-    <row r="2" spans="1:1062" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:1063" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -3354,13 +3369,16 @@
         <v>18710</v>
       </c>
       <c r="BR2" s="3">
-        <f>SUM(BQ2)</f>
-        <v>18710</v>
+        <v>46256</v>
+      </c>
+      <c r="BS2" s="3">
+        <f>SUM(BQ2:BR2)</f>
+        <v>64966</v>
       </c>
     </row>
-    <row r="3" spans="1:1062" x14ac:dyDescent="0.2">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
+    <row r="3" spans="1:1063" x14ac:dyDescent="0.2">
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
       <c r="C3" s="7" t="s">
         <v>29</v>
       </c>
@@ -3561,20 +3579,23 @@
         <v>0</v>
       </c>
       <c r="BP3" s="3">
-        <f t="shared" ref="BP3:BR16" si="4">SUM(BD3:BO3)</f>
+        <f t="shared" ref="BP3:BP16" si="4">SUM(BD3:BO3)</f>
         <v>0</v>
       </c>
       <c r="BQ3" s="3">
         <v>0</v>
       </c>
       <c r="BR3" s="3">
-        <f t="shared" ref="BR3:BR9" si="5">SUM(BQ3)</f>
+        <v>0</v>
+      </c>
+      <c r="BS3" s="3">
+        <f t="shared" ref="BS3:BS16" si="5">SUM(BQ3:BR3)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1062" x14ac:dyDescent="0.2">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
+    <row r="4" spans="1:1063" x14ac:dyDescent="0.2">
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="7" t="s">
         <v>30</v>
       </c>
@@ -3783,13 +3804,16 @@
         <v>0</v>
       </c>
       <c r="BR4" s="3">
+        <v>1730</v>
+      </c>
+      <c r="BS4" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1730</v>
       </c>
     </row>
-    <row r="5" spans="1:1062" x14ac:dyDescent="0.2">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
+    <row r="5" spans="1:1063" x14ac:dyDescent="0.2">
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="7" t="s">
         <v>31</v>
       </c>
@@ -3997,13 +4021,16 @@
         <v>0</v>
       </c>
       <c r="BR5" s="3">
+        <v>0</v>
+      </c>
+      <c r="BS5" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:1062" x14ac:dyDescent="0.2">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
+    <row r="6" spans="1:1063" x14ac:dyDescent="0.2">
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="7" t="s">
         <v>32</v>
       </c>
@@ -4211,13 +4238,16 @@
         <v>0</v>
       </c>
       <c r="BR6" s="3">
+        <v>0</v>
+      </c>
+      <c r="BS6" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:1062" x14ac:dyDescent="0.2">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
+    <row r="7" spans="1:1063" x14ac:dyDescent="0.2">
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="7" t="s">
         <v>33</v>
       </c>
@@ -4425,13 +4455,16 @@
         <v>0</v>
       </c>
       <c r="BR7" s="3">
+        <v>0</v>
+      </c>
+      <c r="BS7" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:1062" x14ac:dyDescent="0.2">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
+    <row r="8" spans="1:1063" x14ac:dyDescent="0.2">
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="7" t="s">
         <v>34</v>
       </c>
@@ -4639,13 +4672,16 @@
         <v>0</v>
       </c>
       <c r="BR8" s="3">
+        <v>0</v>
+      </c>
+      <c r="BS8" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:1062" x14ac:dyDescent="0.2">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
+    <row r="9" spans="1:1063" x14ac:dyDescent="0.2">
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="7" t="s">
         <v>35</v>
       </c>
@@ -4910,17 +4946,21 @@
         <v>234426.71</v>
       </c>
       <c r="BQ9" s="3">
-        <f t="shared" ref="BQ9" si="11">SUM(BQ2:BQ8)</f>
+        <f t="shared" ref="BQ9:BR9" si="11">SUM(BQ2:BQ8)</f>
         <v>18710</v>
       </c>
       <c r="BR9" s="3">
+        <f t="shared" si="11"/>
+        <v>47986</v>
+      </c>
+      <c r="BS9" s="3">
         <f t="shared" si="5"/>
-        <v>18710</v>
+        <v>66696</v>
       </c>
     </row>
-    <row r="10" spans="1:1062" x14ac:dyDescent="0.2">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12" t="s">
+    <row r="10" spans="1:1063" x14ac:dyDescent="0.2">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13" t="s">
         <v>36</v>
       </c>
       <c r="C10" s="7" t="s">
@@ -5131,13 +5171,16 @@
         <v>2447.1</v>
       </c>
       <c r="BR10" s="3">
-        <f>SUM(BQ10)</f>
-        <v>2447.1</v>
+        <v>4317.9799999999996</v>
+      </c>
+      <c r="BS10" s="3">
+        <f t="shared" si="5"/>
+        <v>6765.08</v>
       </c>
     </row>
-    <row r="11" spans="1:1062" x14ac:dyDescent="0.2">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
+    <row r="11" spans="1:1063" x14ac:dyDescent="0.2">
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="7" t="s">
         <v>38</v>
       </c>
@@ -5345,13 +5388,16 @@
         <v>0</v>
       </c>
       <c r="BR11" s="3">
-        <f>SUM(BQ11)</f>
+        <v>0</v>
+      </c>
+      <c r="BS11" s="3">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:1062" x14ac:dyDescent="0.2">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
+    <row r="12" spans="1:1063" x14ac:dyDescent="0.2">
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
       <c r="C12" s="7" t="s">
         <v>39</v>
       </c>
@@ -5560,13 +5606,16 @@
         <v>350.58</v>
       </c>
       <c r="BR12" s="3">
-        <f>SUM(BQ12)</f>
-        <v>350.58</v>
+        <v>462.12</v>
+      </c>
+      <c r="BS12" s="3">
+        <f t="shared" si="5"/>
+        <v>812.7</v>
       </c>
     </row>
-    <row r="13" spans="1:1062" x14ac:dyDescent="0.2">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
+    <row r="13" spans="1:1063" x14ac:dyDescent="0.2">
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
       <c r="C13" s="7" t="s">
         <v>40</v>
       </c>
@@ -5774,13 +5823,16 @@
         <v>0</v>
       </c>
       <c r="BR13" s="3">
-        <f>SUM(BQ13)</f>
+        <v>0</v>
+      </c>
+      <c r="BS13" s="3">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:1062" x14ac:dyDescent="0.2">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
+    <row r="14" spans="1:1063" x14ac:dyDescent="0.2">
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
       <c r="C14" s="7" t="s">
         <v>41</v>
       </c>
@@ -5988,13 +6040,16 @@
         <v>0</v>
       </c>
       <c r="BR14" s="3">
-        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="BS14" s="3">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:1062" x14ac:dyDescent="0.2">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
+    <row r="15" spans="1:1063" x14ac:dyDescent="0.2">
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
       <c r="C15" s="7" t="s">
         <v>35</v>
       </c>
@@ -6259,20 +6314,24 @@
         <v>120487.48999999999</v>
       </c>
       <c r="BQ15" s="3">
-        <f t="shared" ref="BQ15" si="17">SUM(BQ10:BQ14)</f>
+        <f t="shared" ref="BQ15:BR15" si="17">SUM(BQ10:BQ14)</f>
         <v>2797.68</v>
       </c>
       <c r="BR15" s="3">
-        <f>SUM(BQ15)</f>
-        <v>2797.68</v>
+        <f t="shared" si="17"/>
+        <v>4780.0999999999995</v>
+      </c>
+      <c r="BS15" s="3">
+        <f t="shared" si="5"/>
+        <v>7577.7799999999988</v>
       </c>
     </row>
-    <row r="16" spans="1:1062" x14ac:dyDescent="0.2">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12" t="s">
+    <row r="16" spans="1:1063" x14ac:dyDescent="0.2">
+      <c r="A16" s="13"/>
+      <c r="B16" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="12"/>
+      <c r="C16" s="13"/>
       <c r="D16" s="3">
         <f t="shared" ref="D16:O16" si="18">D9-D15</f>
         <v>854.77999999999975</v>
@@ -6534,19 +6593,23 @@
         <v>113939.22</v>
       </c>
       <c r="BQ16" s="3">
-        <f t="shared" ref="BQ16" si="23">BQ9-BQ15</f>
+        <f t="shared" ref="BQ16:BR16" si="23">BQ9-BQ15</f>
         <v>15912.32</v>
       </c>
       <c r="BR16" s="3">
-        <f>SUM(BQ16)</f>
-        <v>15912.32</v>
+        <f t="shared" si="23"/>
+        <v>43205.9</v>
+      </c>
+      <c r="BS16" s="3">
+        <f t="shared" si="5"/>
+        <v>59118.22</v>
       </c>
     </row>
-    <row r="17" spans="1:69" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
+    <row r="17" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A17" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="13" t="s">
         <v>44</v>
       </c>
       <c r="C17" s="7" t="s">
@@ -6736,10 +6799,13 @@
       <c r="BQ17" s="3">
         <v>0</v>
       </c>
+      <c r="BR17" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:69" x14ac:dyDescent="0.2">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
+    <row r="18" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
       <c r="C18" s="7" t="s">
         <v>46</v>
       </c>
@@ -6928,10 +6994,13 @@
       <c r="BQ18" s="3">
         <v>332800</v>
       </c>
+      <c r="BR18" s="3">
+        <v>378800</v>
+      </c>
     </row>
-    <row r="19" spans="1:69" x14ac:dyDescent="0.2">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
+    <row r="19" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
       <c r="C19" s="7" t="s">
         <v>47</v>
       </c>
@@ -7119,10 +7188,13 @@
       <c r="BQ19" s="3">
         <v>33516.69</v>
       </c>
+      <c r="BR19" s="3">
+        <v>33816.69</v>
+      </c>
     </row>
-    <row r="20" spans="1:69" x14ac:dyDescent="0.2">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
+    <row r="20" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
       <c r="C20" s="7" t="s">
         <v>48</v>
       </c>
@@ -7310,10 +7382,13 @@
       <c r="BQ20" s="3">
         <v>6526.8</v>
       </c>
+      <c r="BR20" s="3">
+        <v>6615</v>
+      </c>
     </row>
-    <row r="21" spans="1:69" x14ac:dyDescent="0.2">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
+    <row r="21" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
       <c r="C21" s="7" t="s">
         <v>49</v>
       </c>
@@ -7501,10 +7576,13 @@
       <c r="BQ21" s="3">
         <v>0</v>
       </c>
+      <c r="BR21" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:69" x14ac:dyDescent="0.2">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
+    <row r="22" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A22" s="13"/>
+      <c r="B22" s="13"/>
       <c r="C22" s="7" t="s">
         <v>50</v>
       </c>
@@ -7692,10 +7770,13 @@
       <c r="BQ22" s="3">
         <v>373036.11</v>
       </c>
+      <c r="BR22" s="3">
+        <v>379811.35</v>
+      </c>
     </row>
-    <row r="23" spans="1:69" x14ac:dyDescent="0.2">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
+    <row r="23" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A23" s="13"/>
+      <c r="B23" s="13"/>
       <c r="C23" s="7" t="s">
         <v>35</v>
       </c>
@@ -7940,12 +8021,16 @@
         <v>721854.28</v>
       </c>
       <c r="BQ23" s="8">
-        <f t="shared" ref="BQ23" si="29">SUM(BQ17:BQ22)</f>
+        <f t="shared" ref="BQ23:BR23" si="29">SUM(BQ17:BQ22)</f>
         <v>745879.6</v>
       </c>
+      <c r="BR23" s="8">
+        <f t="shared" si="29"/>
+        <v>799043.04</v>
+      </c>
     </row>
-    <row r="24" spans="1:69" x14ac:dyDescent="0.2">
-      <c r="A24" s="12"/>
+    <row r="24" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A24" s="13"/>
       <c r="B24" s="7" t="s">
         <v>51</v>
       </c>
@@ -8148,7 +8233,7 @@
         <v>156000</v>
       </c>
       <c r="BE24" s="3">
-        <f t="shared" ref="BE24:BQ24" si="34">BD24+BE8-BE14</f>
+        <f t="shared" ref="BE24:BO24" si="34">BD24+BE8-BE14</f>
         <v>156000</v>
       </c>
       <c r="BF24" s="3">
@@ -8195,13 +8280,17 @@
         <f>BO24+BQ8-BQ14</f>
         <v>156000</v>
       </c>
+      <c r="BR24" s="3">
+        <f>BQ24+BR8-BQ14</f>
+        <v>156000</v>
+      </c>
     </row>
-    <row r="25" spans="1:69" x14ac:dyDescent="0.2">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12" t="s">
+    <row r="25" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A25" s="13"/>
+      <c r="B25" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="12"/>
+      <c r="C25" s="13"/>
       <c r="D25" s="8">
         <f t="shared" ref="D25:O25" si="35">D23-D24</f>
         <v>39892.050000000003</v>
@@ -8443,8 +8532,12 @@
         <v>565854.28</v>
       </c>
       <c r="BQ25" s="8">
-        <f t="shared" ref="BQ25" si="40">BQ23-BQ24</f>
+        <f t="shared" ref="BQ25:BR25" si="40">BQ23-BQ24</f>
         <v>589879.6</v>
+      </c>
+      <c r="BR25" s="8">
+        <f t="shared" si="40"/>
+        <v>643043.04</v>
       </c>
     </row>
   </sheetData>

</xml_diff>